<commit_message>
Iterate offline keying template
Change-Id: Ia39e8e5d044563a9369982f607e17ce8e009bc99
</commit_message>
<xml_diff>
--- a/sites/all/modules/offline2civicrm/templates/Individual - Hand Key Import Template.xlsx
+++ b/sites/all/modules/offline2civicrm/templates/Individual - Hand Key Import Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16260" tabRatio="105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="105"/>
   </bookViews>
   <sheets>
     <sheet name="Individual  - Hand Key Import T" sheetId="1" r:id="rId1"/>
@@ -2398,8 +2398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AM6" sqref="AM6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2663,21 +2663,17 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
+  <dataValidations count="13">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B2">
       <formula1>"Cash,Stock,In Kind,Engage"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="D2">
-      <formula1>0</formula1>
-    </dataValidation>
+    <dataValidation operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="D2"/>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2">
       <formula1>3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 AE2">
-      <formula1>42005</formula1>
-    </dataValidation>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2"/>
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G2">
       <formula1>"EFT,JP Morgan,Stock,Check,Cash,UKFC,Bitcoin"</formula1>
       <formula2>0</formula2>
@@ -2704,9 +2700,8 @@
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="M2">
       <formula1>$AZ$2:$AZ$14</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
-      <formula1>40179</formula1>
-    </dataValidation>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2"/>
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2"/>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Provide Generic Org import
Bug: T88836
Change-Id: I227226f7847f9ae223fe0fa6c8b0e2d1babbba89
</commit_message>
<xml_diff>
--- a/sites/all/modules/offline2civicrm/templates/Individual - Hand Key Import Template.xlsx
+++ b/sites/all/modules/offline2civicrm/templates/Individual - Hand Key Import Template.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Individual  - Hand Key Import T" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -361,7 +361,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Target of the relationship.</t>
+          <t>Target of the relationship, by numeric CiviCRM contact ID.</t>
         </r>
       </text>
     </comment>
@@ -515,9 +515,6 @@
     <t>Relationship Type</t>
   </si>
   <si>
-    <t>Target Contact</t>
-  </si>
-  <si>
     <t>Tags</t>
   </si>
   <si>
@@ -582,13 +579,16 @@
   </si>
   <si>
     <t>Do Not Solicit</t>
+  </si>
+  <si>
+    <t>Target Contact ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -605,6 +605,22 @@
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -627,13 +643,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2398,8 +2422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2442,7 +2466,7 @@
     <col min="38" max="38" width="10.5" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="9" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="12" customWidth="1"/>
     <col min="43" max="43" width="12.6640625" customWidth="1"/>
     <col min="52" max="53" width="0" hidden="1" customWidth="1"/>
@@ -2549,7 +2573,7 @@
         <v>32</v>
       </c>
       <c r="AH1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI1" t="s">
         <v>33</v>
@@ -2570,96 +2594,96 @@
         <v>38</v>
       </c>
       <c r="AO1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>40</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:53">
       <c r="AZ2" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA2" t="s">
         <v>42</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:53">
       <c r="AZ3" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA3" t="s">
         <v>44</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:53">
       <c r="AZ4" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA4" t="s">
         <v>46</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:53">
       <c r="AZ5" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA5" t="s">
         <v>48</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:53">
       <c r="AZ6" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA6" t="s">
         <v>50</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:53">
       <c r="AZ7" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA7" t="s">
         <v>52</v>
-      </c>
-      <c r="BA7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:53">
       <c r="AZ8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:53">
       <c r="AZ9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:53">
       <c r="AZ10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:53">
       <c r="AZ11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:53">
       <c r="AZ12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:53">
       <c r="AZ13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:53">
       <c r="AZ14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>